<commit_message>
working on serving CMM Upload file to user through UI
</commit_message>
<xml_diff>
--- a/utils/Templates/Measurement_Import_Template.xlsx
+++ b/utils/Templates/Measurement_Import_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Desktop\import and export\Latest templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccoats\Desktop\python\KPC Manager\KPC_Manager2\utils\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D387A3D-5948-4169-9242-6E4563A8AA9E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C0931B2-D001-4A0A-A935-E220320C15A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9588" tabRatio="855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11925" tabRatio="855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Measurements" sheetId="6724" r:id="rId1"/>
@@ -472,30 +472,30 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="4" customWidth="1"/>
     <col min="8" max="8" width="14" style="4" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="4"/>
+    <col min="9" max="9" width="19.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="4"/>
     <col min="12" max="12" width="10" style="4" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.44140625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="2"/>
+    <col min="13" max="13" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
@@ -540,39 +540,39 @@
       </c>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="C2" s="3"/>
       <c r="F2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="C3" s="3"/>
       <c r="F3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="C4" s="3"/>
       <c r="F4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="C5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="C6" s="3"/>
       <c r="F6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C9" s="3"/>
     </row>
   </sheetData>

</xml_diff>